<commit_message>
various changes to ref deisgnators and OOI barcodes
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP03FLMA_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\IRAD\IRAD 2015\Programs\OOI Phase 2\Post Delivery 7 support\Asset Management Data\ingestion-csvs_20151204\ingestion-csvs\GP03FLMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10716" yWindow="7716" windowWidth="24960" windowHeight="12624" activeTab="1"/>
+    <workbookView xWindow="10710" yWindow="7710" windowWidth="24960" windowHeight="12630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -198,48 +198,6 @@
     <t>GP03FLMA-RIM01-02-ADCPSL003</t>
   </si>
   <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG057</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG020</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG060</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG015</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG054</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG062</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG052</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG019</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOG056</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOH026</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOH029</t>
-  </si>
-  <si>
-    <t>GP03FLMA-RIM01-02-CTDMOH067</t>
-  </si>
-  <si>
-    <t>GP03FLMA-00001-FMM01</t>
-  </si>
-  <si>
-    <t>GP03FLMA-00001-FMS01</t>
-  </si>
-  <si>
     <t>This serial number is made up until we can find the real serial number</t>
   </si>
   <si>
@@ -400,6 +358,48 @@
   </si>
   <si>
     <t>A00152</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOH051</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOH050</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOH049</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG048</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG047</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG046</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG045</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG044</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG043</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG042</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG041</t>
+  </si>
+  <si>
+    <t>GP03FLMA-RIM01-02-CTDMOG040</t>
+  </si>
+  <si>
+    <t>OL000080</t>
+  </si>
+  <si>
+    <t>OL000021</t>
   </si>
 </sst>
 </file>
@@ -1157,24 +1157,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="9" customWidth="1"/>
     <col min="3" max="3" width="16" style="9" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="11" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" style="9" customWidth="1"/>
-    <col min="10" max="11" width="8.77734375" style="9"/>
-    <col min="12" max="12" width="44.109375" style="9" customWidth="1"/>
-    <col min="13" max="1026" width="8.77734375" style="9"/>
+    <col min="4" max="4" width="9.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="11" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" style="9" customWidth="1"/>
+    <col min="10" max="11" width="8.7109375" style="9"/>
+    <col min="12" max="12" width="44.140625" style="9" customWidth="1"/>
+    <col min="13" max="1026" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="20" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="20" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -1214,9 +1214,9 @@
       <c r="O1" s="19"/>
       <c r="P1" s="19"/>
     </row>
-    <row r="2" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>11</v>
@@ -1237,19 +1237,19 @@
         <v>41805</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="I2" s="54" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="J2" s="22">
         <v>4127</v>
       </c>
       <c r="K2" s="55" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
@@ -1272,30 +1272,30 @@
   <dimension ref="A1:AMM98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C100" sqref="C100"/>
+      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" style="29" customWidth="1"/>
-    <col min="2" max="3" width="15.77734375" style="29" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" style="29" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" style="29" customWidth="1"/>
     <col min="4" max="5" width="11" style="30" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="31.44140625" style="29" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="29" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" style="29" customWidth="1"/>
     <col min="9" max="9" width="17" style="30" customWidth="1"/>
-    <col min="10" max="1027" width="8.77734375" style="29"/>
+    <col min="10" max="1027" width="8.7109375" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" s="36" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1026" s="36" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>13</v>
@@ -1304,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>14</v>
@@ -1325,7 +1325,7 @@
       <c r="N1" s="35"/>
       <c r="O1" s="35"/>
     </row>
-    <row r="2" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -2353,12 +2353,12 @@
       <c r="AMK2"/>
       <c r="AML2"/>
     </row>
-    <row r="3" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>12</v>
@@ -2367,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F3" s="22">
         <v>1005</v>
@@ -3401,12 +3401,12 @@
       <c r="AMK3"/>
       <c r="AML3"/>
     </row>
-    <row r="4" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>12</v>
@@ -3415,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F4" s="41">
         <v>1005</v>
@@ -4447,12 +4447,12 @@
       <c r="AMK4"/>
       <c r="AML4"/>
     </row>
-    <row r="5" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>12</v>
@@ -4461,7 +4461,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F5" s="41">
         <v>1005</v>
@@ -5491,12 +5491,12 @@
       <c r="AMK5"/>
       <c r="AML5"/>
     </row>
-    <row r="6" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C6" s="41" t="s">
         <v>12</v>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F6" s="41">
         <v>1005</v>
@@ -6535,12 +6535,12 @@
       <c r="AMK6"/>
       <c r="AML6"/>
     </row>
-    <row r="7" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>12</v>
@@ -6549,7 +6549,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F7" s="41">
         <v>1005</v>
@@ -7579,12 +7579,12 @@
       <c r="AMK7"/>
       <c r="AML7"/>
     </row>
-    <row r="8" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C8" s="41" t="s">
         <v>12</v>
@@ -7593,7 +7593,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F8" s="41">
         <v>1005</v>
@@ -8623,12 +8623,12 @@
       <c r="AMK8"/>
       <c r="AML8"/>
     </row>
-    <row r="9" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C9" s="41" t="s">
         <v>12</v>
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F9" s="41">
         <v>1005</v>
@@ -9669,12 +9669,12 @@
       <c r="AMK9"/>
       <c r="AML9"/>
     </row>
-    <row r="10" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>12</v>
@@ -9683,7 +9683,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F10" s="41">
         <v>1005</v>
@@ -10715,12 +10715,12 @@
       <c r="AMK10"/>
       <c r="AML10"/>
     </row>
-    <row r="11" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C11" s="41" t="s">
         <v>12</v>
@@ -10729,7 +10729,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F11" s="41">
         <v>1005</v>
@@ -11761,12 +11761,12 @@
       <c r="AMK11"/>
       <c r="AML11"/>
     </row>
-    <row r="12" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C12" s="41" t="s">
         <v>12</v>
@@ -11775,7 +11775,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F12" s="41">
         <v>1005</v>
@@ -12807,7 +12807,7 @@
       <c r="AMK12"/>
       <c r="AML12"/>
     </row>
-    <row r="13" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A13" s="61"/>
       <c r="B13"/>
       <c r="C13" s="41"/>
@@ -13832,12 +13832,12 @@
       <c r="AMK13"/>
       <c r="AML13"/>
     </row>
-    <row r="14" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
         <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>12</v>
@@ -13846,10 +13846,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G14" s="39" t="s">
         <v>31</v>
@@ -14880,12 +14880,12 @@
       <c r="AMK14"/>
       <c r="AML14"/>
     </row>
-    <row r="15" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>12</v>
@@ -14894,10 +14894,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G15" s="39" t="s">
         <v>32</v>
@@ -15924,12 +15924,12 @@
       <c r="AMK15"/>
       <c r="AML15"/>
     </row>
-    <row r="16" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>12</v>
@@ -15938,10 +15938,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>33</v>
@@ -16968,12 +16968,12 @@
       <c r="AMK16"/>
       <c r="AML16"/>
     </row>
-    <row r="17" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>12</v>
@@ -16982,10 +16982,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>34</v>
@@ -18012,12 +18012,12 @@
       <c r="AMK17"/>
       <c r="AML17"/>
     </row>
-    <row r="18" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>12</v>
@@ -18026,10 +18026,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>35</v>
@@ -19056,12 +19056,12 @@
       <c r="AMK18"/>
       <c r="AML18"/>
     </row>
-    <row r="19" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>12</v>
@@ -19070,10 +19070,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G19" s="43" t="s">
         <v>36</v>
@@ -20100,12 +20100,12 @@
       <c r="AMK19"/>
       <c r="AML19"/>
     </row>
-    <row r="20" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>12</v>
@@ -20114,10 +20114,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G20" s="43" t="s">
         <v>37</v>
@@ -21146,7 +21146,7 @@
       <c r="AMK20"/>
       <c r="AML20"/>
     </row>
-    <row r="21" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21"/>
       <c r="C21" s="22"/>
@@ -22171,12 +22171,12 @@
       <c r="AMK21"/>
       <c r="AML21"/>
     </row>
-    <row r="22" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>12</v>
@@ -22185,7 +22185,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F22" s="22">
         <v>129</v>
@@ -23219,12 +23219,12 @@
       <c r="AMK22"/>
       <c r="AML22"/>
     </row>
-    <row r="23" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C23" s="41" t="s">
         <v>12</v>
@@ -23233,7 +23233,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F23" s="41">
         <v>129</v>
@@ -24265,12 +24265,12 @@
       <c r="AMK23"/>
       <c r="AML23"/>
     </row>
-    <row r="24" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>12</v>
@@ -24279,7 +24279,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F24" s="41">
         <v>129</v>
@@ -25309,7 +25309,7 @@
       <c r="AMK24"/>
       <c r="AML24"/>
     </row>
-    <row r="25" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="40"/>
       <c r="C25" s="41"/>
@@ -26337,12 +26337,12 @@
       <c r="AMK25"/>
       <c r="AML25"/>
     </row>
-    <row r="26" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>12</v>
@@ -26351,7 +26351,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F26" s="22">
         <v>18351</v>
@@ -27385,12 +27385,12 @@
       <c r="AMK26"/>
       <c r="AML26"/>
     </row>
-    <row r="27" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C27" s="41" t="s">
         <v>12</v>
@@ -27399,7 +27399,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F27" s="41">
         <v>18351</v>
@@ -28429,12 +28429,12 @@
       <c r="AMK27"/>
       <c r="AML27"/>
     </row>
-    <row r="28" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C28" s="41" t="s">
         <v>12</v>
@@ -28443,7 +28443,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F28" s="41">
         <v>18351</v>
@@ -29473,12 +29473,12 @@
       <c r="AMK28"/>
       <c r="AML28"/>
     </row>
-    <row r="29" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>12</v>
@@ -29487,7 +29487,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F29" s="41">
         <v>18351</v>
@@ -30517,12 +30517,12 @@
       <c r="AMK29"/>
       <c r="AML29"/>
     </row>
-    <row r="30" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C30" s="41" t="s">
         <v>12</v>
@@ -30531,7 +30531,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F30" s="41">
         <v>18351</v>
@@ -30543,7 +30543,7 @@
         <v>500000</v>
       </c>
       <c r="I30" s="58" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="J30"/>
       <c r="K30"/>
@@ -31563,12 +31563,12 @@
       <c r="AMK30"/>
       <c r="AML30"/>
     </row>
-    <row r="31" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C31" s="41" t="s">
         <v>12</v>
@@ -31577,7 +31577,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F31" s="41">
         <v>18351</v>
@@ -32607,12 +32607,12 @@
       <c r="AMK31"/>
       <c r="AML31"/>
     </row>
-    <row r="32" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C32" s="41" t="s">
         <v>12</v>
@@ -32621,7 +32621,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F32" s="41">
         <v>18351</v>
@@ -33651,12 +33651,12 @@
       <c r="AMK32"/>
       <c r="AML32"/>
     </row>
-    <row r="33" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C33" s="41" t="s">
         <v>12</v>
@@ -33665,7 +33665,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F33" s="41">
         <v>18351</v>
@@ -34695,12 +34695,12 @@
       <c r="AMK33"/>
       <c r="AML33"/>
     </row>
-    <row r="34" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C34" s="41" t="s">
         <v>12</v>
@@ -34709,7 +34709,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F34" s="41">
         <v>18351</v>
@@ -35739,7 +35739,7 @@
       <c r="AMK34"/>
       <c r="AML34"/>
     </row>
-    <row r="35" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35"/>
       <c r="C35" s="41"/>
@@ -36765,12 +36765,12 @@
       <c r="AMK35"/>
       <c r="AML35"/>
     </row>
-    <row r="36" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>57</v>
+    <row r="36" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>12</v>
@@ -36779,10 +36779,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F36" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G36" s="39" t="s">
         <v>52</v>
@@ -37813,12 +37813,12 @@
       <c r="AMK36"/>
       <c r="AML36"/>
     </row>
-    <row r="37" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A37" s="41" t="s">
-        <v>57</v>
+    <row r="37" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C37" s="41" t="s">
         <v>12</v>
@@ -37827,10 +37827,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G37" s="39" t="s">
         <v>40</v>
@@ -38857,12 +38857,12 @@
       <c r="AMK37"/>
       <c r="AML37"/>
     </row>
-    <row r="38" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A38" s="41" t="s">
-        <v>57</v>
+    <row r="38" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C38" s="41" t="s">
         <v>12</v>
@@ -38871,10 +38871,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G38" s="47" t="s">
         <v>41</v>
@@ -39901,12 +39901,12 @@
       <c r="AMK38"/>
       <c r="AML38"/>
     </row>
-    <row r="39" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A39" s="41" t="s">
-        <v>57</v>
+    <row r="39" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>12</v>
@@ -39915,10 +39915,10 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G39" s="39" t="s">
         <v>53</v>
@@ -40945,7 +40945,7 @@
       <c r="AMK39"/>
       <c r="AML39"/>
     </row>
-    <row r="40" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A40" s="61"/>
       <c r="B40"/>
       <c r="C40" s="41"/>
@@ -41971,12 +41971,12 @@
       <c r="AMK40"/>
       <c r="AML40"/>
     </row>
-    <row r="41" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>58</v>
+    <row r="41" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>12</v>
@@ -41985,10 +41985,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G41" s="39" t="s">
         <v>52</v>
@@ -43019,12 +43019,12 @@
       <c r="AMK41"/>
       <c r="AML41"/>
     </row>
-    <row r="42" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A42" s="41" t="s">
-        <v>58</v>
+    <row r="42" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C42" s="41" t="s">
         <v>12</v>
@@ -43033,10 +43033,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G42" s="39" t="s">
         <v>40</v>
@@ -44063,12 +44063,12 @@
       <c r="AMK42"/>
       <c r="AML42"/>
     </row>
-    <row r="43" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A43" s="41" t="s">
-        <v>58</v>
+    <row r="43" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C43" s="41" t="s">
         <v>12</v>
@@ -44077,10 +44077,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G43" s="47" t="s">
         <v>41</v>
@@ -45107,12 +45107,12 @@
       <c r="AMK43"/>
       <c r="AML43"/>
     </row>
-    <row r="44" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A44" s="41" t="s">
-        <v>58</v>
+    <row r="44" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C44" s="41" t="s">
         <v>12</v>
@@ -45121,10 +45121,10 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G44" s="39" t="s">
         <v>53</v>
@@ -46151,7 +46151,7 @@
       <c r="AMK44"/>
       <c r="AML44"/>
     </row>
-    <row r="45" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A45" s="61"/>
       <c r="B45"/>
       <c r="C45" s="41"/>
@@ -47177,12 +47177,12 @@
       <c r="AMK45"/>
       <c r="AML45"/>
     </row>
-    <row r="46" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>59</v>
+    <row r="46" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>12</v>
@@ -47191,10 +47191,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G46" s="39" t="s">
         <v>52</v>
@@ -48225,12 +48225,12 @@
       <c r="AMK46"/>
       <c r="AML46"/>
     </row>
-    <row r="47" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A47" s="41" t="s">
-        <v>59</v>
+    <row r="47" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C47" s="41" t="s">
         <v>12</v>
@@ -48239,10 +48239,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F47" s="41" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G47" s="39" t="s">
         <v>40</v>
@@ -49269,12 +49269,12 @@
       <c r="AMK47"/>
       <c r="AML47"/>
     </row>
-    <row r="48" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A48" s="41" t="s">
-        <v>59</v>
+    <row r="48" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C48" s="41" t="s">
         <v>12</v>
@@ -49283,10 +49283,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F48" s="41" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G48" s="47" t="s">
         <v>41</v>
@@ -50313,12 +50313,12 @@
       <c r="AMK48"/>
       <c r="AML48"/>
     </row>
-    <row r="49" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A49" s="41" t="s">
-        <v>59</v>
+    <row r="49" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C49" s="41" t="s">
         <v>12</v>
@@ -50327,10 +50327,10 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F49" s="41" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G49" s="39" t="s">
         <v>53</v>
@@ -51357,7 +51357,7 @@
       <c r="AMK49"/>
       <c r="AML49"/>
     </row>
-    <row r="50" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A50" s="61"/>
       <c r="B50"/>
       <c r="C50" s="41"/>
@@ -52383,12 +52383,12 @@
       <c r="AMK50"/>
       <c r="AML50"/>
     </row>
-    <row r="51" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
-        <v>60</v>
+    <row r="51" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>105</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>12</v>
@@ -52397,10 +52397,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G51" s="39" t="s">
         <v>52</v>
@@ -53431,12 +53431,12 @@
       <c r="AMK51"/>
       <c r="AML51"/>
     </row>
-    <row r="52" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A52" s="41" t="s">
-        <v>60</v>
+    <row r="52" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C52" s="41" t="s">
         <v>12</v>
@@ -53445,10 +53445,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F52" s="41" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G52" s="39" t="s">
         <v>40</v>
@@ -54475,12 +54475,12 @@
       <c r="AMK52"/>
       <c r="AML52"/>
     </row>
-    <row r="53" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A53" s="41" t="s">
-        <v>60</v>
+    <row r="53" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>12</v>
@@ -54489,10 +54489,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F53" s="41" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G53" s="47" t="s">
         <v>41</v>
@@ -55519,12 +55519,12 @@
       <c r="AMK53"/>
       <c r="AML53"/>
     </row>
-    <row r="54" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A54" s="41" t="s">
-        <v>60</v>
+    <row r="54" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>105</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C54" s="41" t="s">
         <v>12</v>
@@ -55533,10 +55533,10 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F54" s="41" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G54" s="39" t="s">
         <v>53</v>
@@ -56563,7 +56563,7 @@
       <c r="AMK54"/>
       <c r="AML54"/>
     </row>
-    <row r="55" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A55" s="61"/>
       <c r="B55"/>
       <c r="C55" s="41"/>
@@ -57589,12 +57589,12 @@
       <c r="AMK55"/>
       <c r="AML55"/>
     </row>
-    <row r="56" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>61</v>
+    <row r="56" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C56" s="22" t="s">
         <v>12</v>
@@ -57603,10 +57603,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G56" s="39" t="s">
         <v>52</v>
@@ -58637,12 +58637,12 @@
       <c r="AMK56"/>
       <c r="AML56"/>
     </row>
-    <row r="57" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A57" s="41" t="s">
-        <v>61</v>
+    <row r="57" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C57" s="41" t="s">
         <v>12</v>
@@ -58651,10 +58651,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F57" s="41" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G57" s="39" t="s">
         <v>40</v>
@@ -59681,12 +59681,12 @@
       <c r="AMK57"/>
       <c r="AML57"/>
     </row>
-    <row r="58" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A58" s="41" t="s">
-        <v>61</v>
+    <row r="58" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>104</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C58" s="41" t="s">
         <v>12</v>
@@ -59695,10 +59695,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F58" s="41" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G58" s="47" t="s">
         <v>41</v>
@@ -60725,12 +60725,12 @@
       <c r="AMK58"/>
       <c r="AML58"/>
     </row>
-    <row r="59" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A59" s="41" t="s">
-        <v>61</v>
+    <row r="59" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>104</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C59" s="41" t="s">
         <v>12</v>
@@ -60739,10 +60739,10 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F59" s="41" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G59" s="39" t="s">
         <v>53</v>
@@ -61769,7 +61769,7 @@
       <c r="AMK59"/>
       <c r="AML59"/>
     </row>
-    <row r="60" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A60" s="61"/>
       <c r="B60"/>
       <c r="C60" s="41"/>
@@ -62795,12 +62795,12 @@
       <c r="AMK60"/>
       <c r="AML60"/>
     </row>
-    <row r="61" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A61" s="8" t="s">
-        <v>62</v>
+    <row r="61" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>103</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>12</v>
@@ -62809,10 +62809,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G61" s="39" t="s">
         <v>52</v>
@@ -63843,12 +63843,12 @@
       <c r="AMK61"/>
       <c r="AML61"/>
     </row>
-    <row r="62" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A62" s="41" t="s">
-        <v>62</v>
+    <row r="62" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C62" s="41" t="s">
         <v>12</v>
@@ -63857,10 +63857,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F62" s="41" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G62" s="39" t="s">
         <v>40</v>
@@ -64887,12 +64887,12 @@
       <c r="AMK62"/>
       <c r="AML62"/>
     </row>
-    <row r="63" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A63" s="41" t="s">
-        <v>62</v>
+    <row r="63" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C63" s="41" t="s">
         <v>12</v>
@@ -64901,10 +64901,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F63" s="41" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G63" s="47" t="s">
         <v>41</v>
@@ -65931,12 +65931,12 @@
       <c r="AMK63"/>
       <c r="AML63"/>
     </row>
-    <row r="64" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A64" s="41" t="s">
-        <v>62</v>
+    <row r="64" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C64" s="41" t="s">
         <v>12</v>
@@ -65945,10 +65945,10 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G64" s="39" t="s">
         <v>53</v>
@@ -66975,7 +66975,7 @@
       <c r="AMK64"/>
       <c r="AML64"/>
     </row>
-    <row r="65" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A65" s="61"/>
       <c r="B65"/>
       <c r="C65" s="41"/>
@@ -68001,12 +68001,12 @@
       <c r="AMK65"/>
       <c r="AML65"/>
     </row>
-    <row r="66" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A66" s="8" t="s">
-        <v>63</v>
+    <row r="66" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>102</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>12</v>
@@ -68015,10 +68015,10 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G66" s="39" t="s">
         <v>52</v>
@@ -69049,12 +69049,12 @@
       <c r="AMK66"/>
       <c r="AML66"/>
     </row>
-    <row r="67" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A67" s="41" t="s">
-        <v>63</v>
+    <row r="67" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>102</v>
       </c>
       <c r="B67" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C67" s="41" t="s">
         <v>12</v>
@@ -69063,10 +69063,10 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G67" s="39" t="s">
         <v>40</v>
@@ -70093,12 +70093,12 @@
       <c r="AMK67"/>
       <c r="AML67"/>
     </row>
-    <row r="68" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A68" s="41" t="s">
-        <v>63</v>
+    <row r="68" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C68" s="41" t="s">
         <v>12</v>
@@ -70107,10 +70107,10 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G68" s="47" t="s">
         <v>41</v>
@@ -71137,12 +71137,12 @@
       <c r="AMK68"/>
       <c r="AML68"/>
     </row>
-    <row r="69" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A69" s="41" t="s">
-        <v>63</v>
+    <row r="69" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>102</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C69" s="41" t="s">
         <v>12</v>
@@ -71151,10 +71151,10 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G69" s="39" t="s">
         <v>53</v>
@@ -72181,7 +72181,7 @@
       <c r="AMK69"/>
       <c r="AML69"/>
     </row>
-    <row r="70" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A70" s="61"/>
       <c r="B70"/>
       <c r="C70" s="41"/>
@@ -73207,12 +73207,12 @@
       <c r="AMK70"/>
       <c r="AML70"/>
     </row>
-    <row r="71" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A71" s="8" t="s">
-        <v>64</v>
+    <row r="71" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>101</v>
       </c>
       <c r="B71" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>12</v>
@@ -73221,10 +73221,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F71" s="22" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G71" s="39" t="s">
         <v>52</v>
@@ -74255,12 +74255,12 @@
       <c r="AMK71"/>
       <c r="AML71"/>
     </row>
-    <row r="72" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A72" s="41" t="s">
-        <v>64</v>
+    <row r="72" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C72" s="41" t="s">
         <v>12</v>
@@ -74269,10 +74269,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G72" s="39" t="s">
         <v>40</v>
@@ -75299,12 +75299,12 @@
       <c r="AMK72"/>
       <c r="AML72"/>
     </row>
-    <row r="73" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A73" s="41" t="s">
-        <v>64</v>
+    <row r="73" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>101</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C73" s="41" t="s">
         <v>12</v>
@@ -75313,10 +75313,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G73" s="47" t="s">
         <v>41</v>
@@ -76343,12 +76343,12 @@
       <c r="AMK73"/>
       <c r="AML73"/>
     </row>
-    <row r="74" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A74" s="41" t="s">
-        <v>64</v>
+    <row r="74" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>101</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C74" s="41" t="s">
         <v>12</v>
@@ -76357,10 +76357,10 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G74" s="39" t="s">
         <v>53</v>
@@ -77387,7 +77387,7 @@
       <c r="AMK74"/>
       <c r="AML74"/>
     </row>
-    <row r="75" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A75" s="61"/>
       <c r="B75"/>
       <c r="C75" s="41"/>
@@ -78413,12 +78413,12 @@
       <c r="AMK75"/>
       <c r="AML75"/>
     </row>
-    <row r="76" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A76" s="8" t="s">
-        <v>65</v>
+    <row r="76" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C76" s="22" t="s">
         <v>12</v>
@@ -78427,10 +78427,10 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F76" s="22" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="G76" s="39" t="s">
         <v>52</v>
@@ -79461,12 +79461,12 @@
       <c r="AMK76"/>
       <c r="AML76"/>
     </row>
-    <row r="77" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A77" s="41" t="s">
-        <v>65</v>
+    <row r="77" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C77" s="41" t="s">
         <v>12</v>
@@ -79475,10 +79475,10 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F77" s="41" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="G77" s="39" t="s">
         <v>40</v>
@@ -80505,12 +80505,12 @@
       <c r="AMK77"/>
       <c r="AML77"/>
     </row>
-    <row r="78" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A78" s="41" t="s">
-        <v>65</v>
+    <row r="78" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>100</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C78" s="41" t="s">
         <v>12</v>
@@ -80519,10 +80519,10 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F78" s="41" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="G78" s="47" t="s">
         <v>41</v>
@@ -81549,12 +81549,12 @@
       <c r="AMK78"/>
       <c r="AML78"/>
     </row>
-    <row r="79" spans="1:1026" x14ac:dyDescent="0.3">
-      <c r="A79" s="41" t="s">
-        <v>65</v>
+    <row r="79" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>100</v>
       </c>
       <c r="B79" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C79" s="41" t="s">
         <v>12</v>
@@ -81563,10 +81563,10 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F79" s="41" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="G79" s="39" t="s">
         <v>53</v>
@@ -82593,7 +82593,7 @@
       <c r="AMK79"/>
       <c r="AML79"/>
     </row>
-    <row r="80" spans="1:1026" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A80" s="61"/>
       <c r="B80"/>
       <c r="C80" s="41"/>
@@ -83619,12 +83619,12 @@
       <c r="AMK80"/>
       <c r="AML80"/>
     </row>
-    <row r="81" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="8" t="s">
-        <v>66</v>
+    <row r="81" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>99</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C81" s="48" t="s">
         <v>12</v>
@@ -83633,10 +83633,10 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F81" s="48" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G81" s="49" t="s">
         <v>52</v>
@@ -83652,12 +83652,12 @@
       </c>
       <c r="L81" s="48"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" s="41" t="s">
-        <v>66</v>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>99</v>
       </c>
       <c r="B82" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C82" s="52" t="s">
         <v>12</v>
@@ -83666,10 +83666,10 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F82" s="52" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G82" s="39" t="s">
         <v>40</v>
@@ -83681,12 +83681,12 @@
       <c r="J82"/>
       <c r="L82" s="22"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="41" t="s">
-        <v>66</v>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>99</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C83" s="52" t="s">
         <v>12</v>
@@ -83695,10 +83695,10 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F83" s="52" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G83" s="47" t="s">
         <v>41</v>
@@ -83710,12 +83710,12 @@
       <c r="J83"/>
       <c r="L83" s="22"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" s="41" t="s">
-        <v>66</v>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>99</v>
       </c>
       <c r="B84" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C84" s="52" t="s">
         <v>12</v>
@@ -83724,10 +83724,10 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F84" s="52" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G84" s="39" t="s">
         <v>53</v>
@@ -83739,7 +83739,7 @@
       <c r="J84"/>
       <c r="L84" s="22"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="61"/>
       <c r="B85"/>
       <c r="C85" s="52"/>
@@ -83750,12 +83750,12 @@
       <c r="J85"/>
       <c r="L85" s="22"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" s="8" t="s">
-        <v>67</v>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>98</v>
       </c>
       <c r="B86" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C86" s="22" t="s">
         <v>12</v>
@@ -83764,10 +83764,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F86" s="22" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G86" s="39" t="s">
         <v>52</v>
@@ -83783,12 +83783,12 @@
       </c>
       <c r="L86" s="22"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A87" s="41" t="s">
-        <v>67</v>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>98</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C87" s="41" t="s">
         <v>12</v>
@@ -83797,10 +83797,10 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F87" s="41" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G87" s="39" t="s">
         <v>40</v>
@@ -83812,12 +83812,12 @@
       <c r="J87"/>
       <c r="L87" s="22"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A88" s="41" t="s">
-        <v>67</v>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C88" s="41" t="s">
         <v>12</v>
@@ -83826,10 +83826,10 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F88" s="41" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G88" s="47" t="s">
         <v>41</v>
@@ -83841,12 +83841,12 @@
       <c r="J88"/>
       <c r="L88" s="22"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A89" s="41" t="s">
-        <v>67</v>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>98</v>
       </c>
       <c r="B89" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C89" s="41" t="s">
         <v>12</v>
@@ -83855,10 +83855,10 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F89" s="41" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G89" s="39" t="s">
         <v>53</v>
@@ -83870,7 +83870,7 @@
       <c r="J89"/>
       <c r="L89" s="22"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="61"/>
       <c r="B90"/>
       <c r="C90" s="41"/>
@@ -83881,12 +83881,12 @@
       <c r="J90"/>
       <c r="L90" s="22"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A91" s="8" t="s">
-        <v>68</v>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C91" s="22" t="s">
         <v>12</v>
@@ -83895,10 +83895,10 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F91" s="22" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G91" s="39" t="s">
         <v>52</v>
@@ -83914,12 +83914,12 @@
       </c>
       <c r="L91" s="22"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A92" s="41" t="s">
-        <v>68</v>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C92" s="41" t="s">
         <v>12</v>
@@ -83928,10 +83928,10 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F92" s="41" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G92" s="39" t="s">
         <v>40</v>
@@ -83941,12 +83941,12 @@
       </c>
       <c r="L92" s="22"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="41" t="s">
-        <v>68</v>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C93" s="41" t="s">
         <v>12</v>
@@ -83955,10 +83955,10 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F93" s="41" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G93" s="47" t="s">
         <v>41</v>
@@ -83968,12 +83968,12 @@
       </c>
       <c r="L93" s="22"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="41" t="s">
-        <v>68</v>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C94" s="41" t="s">
         <v>12</v>
@@ -83982,10 +83982,10 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F94" s="41" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G94" s="39" t="s">
         <v>53</v>
@@ -83995,15 +83995,15 @@
       </c>
       <c r="L94" s="22"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L95" s="22"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B96" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>12</v>
@@ -84011,15 +84011,17 @@
       <c r="D96" s="4">
         <v>1</v>
       </c>
-      <c r="E96" s="4"/>
-      <c r="F96" s="3" t="s">
-        <v>69</v>
+      <c r="E96" t="s">
+        <v>109</v>
+      </c>
+      <c r="F96" s="3">
+        <v>11690</v>
       </c>
       <c r="I96" s="25" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="62"/>
       <c r="B97" s="63"/>
       <c r="C97" s="22"/>
@@ -84028,12 +84030,12 @@
       <c r="F97" s="65"/>
       <c r="I97" s="25"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B98" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>12</v>
@@ -84041,12 +84043,14 @@
       <c r="D98" s="4">
         <v>1</v>
       </c>
-      <c r="E98" s="4"/>
-      <c r="F98" s="3" t="s">
-        <v>70</v>
+      <c r="E98" t="s">
+        <v>110</v>
+      </c>
+      <c r="F98" s="3">
+        <v>12372</v>
       </c>
       <c r="I98" s="25" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed engineering ref designators
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP03FLMA_00001.xlsx
@@ -216,54 +216,6 @@
     <t>Units in mm</t>
   </si>
   <si>
-    <r>
-      <t>GP03FLMA-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>RI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>M01-01-SIOENG000</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>GP03FLMA-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>RI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>S01-01-SIOENG000</t>
-    </r>
-  </si>
-  <si>
     <t>Mooring OOIBARCODE</t>
   </si>
   <si>
@@ -400,6 +352,54 @@
   </si>
   <si>
     <t>OL000021</t>
+  </si>
+  <si>
+    <r>
+      <t>GP03FLMA-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>M01-00-SIOENG000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GP03FLMA-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>S01-00-SIOENG000</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1174,7 +1174,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="20" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="2" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>11</v>
@@ -1272,10 +1272,10 @@
   <dimension ref="A1:AMM98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
+      <selection pane="bottomRight" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>13</v>
@@ -1304,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>14</v>
@@ -2358,7 +2358,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>12</v>
@@ -2367,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3" s="22">
         <v>1005</v>
@@ -3406,7 +3406,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>12</v>
@@ -3415,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="41">
         <v>1005</v>
@@ -4452,7 +4452,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>12</v>
@@ -4461,7 +4461,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="41">
         <v>1005</v>
@@ -5496,7 +5496,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="41" t="s">
         <v>12</v>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="41">
         <v>1005</v>
@@ -6540,7 +6540,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>12</v>
@@ -6549,7 +6549,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" s="41">
         <v>1005</v>
@@ -7584,7 +7584,7 @@
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="41" t="s">
         <v>12</v>
@@ -7593,7 +7593,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" s="41">
         <v>1005</v>
@@ -8628,7 +8628,7 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="41" t="s">
         <v>12</v>
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="41">
         <v>1005</v>
@@ -9674,7 +9674,7 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>12</v>
@@ -9683,7 +9683,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" s="41">
         <v>1005</v>
@@ -10720,7 +10720,7 @@
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" s="41" t="s">
         <v>12</v>
@@ -10729,7 +10729,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" s="41">
         <v>1005</v>
@@ -11766,7 +11766,7 @@
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="41" t="s">
         <v>12</v>
@@ -11775,7 +11775,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" s="41">
         <v>1005</v>
@@ -13837,7 +13837,7 @@
         <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>12</v>
@@ -13846,10 +13846,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G14" s="39" t="s">
         <v>31</v>
@@ -14885,7 +14885,7 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>12</v>
@@ -14894,10 +14894,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G15" s="39" t="s">
         <v>32</v>
@@ -15929,7 +15929,7 @@
         <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>12</v>
@@ -15938,10 +15938,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>33</v>
@@ -16973,7 +16973,7 @@
         <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>12</v>
@@ -16982,10 +16982,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>34</v>
@@ -18017,7 +18017,7 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>12</v>
@@ -18026,10 +18026,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>35</v>
@@ -19061,7 +19061,7 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>12</v>
@@ -19070,10 +19070,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G19" s="43" t="s">
         <v>36</v>
@@ -20105,7 +20105,7 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>12</v>
@@ -20114,10 +20114,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G20" s="43" t="s">
         <v>37</v>
@@ -22176,7 +22176,7 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>12</v>
@@ -22185,7 +22185,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F22" s="22">
         <v>129</v>
@@ -23224,7 +23224,7 @@
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="41" t="s">
         <v>12</v>
@@ -23233,7 +23233,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" s="41">
         <v>129</v>
@@ -24270,7 +24270,7 @@
         <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>12</v>
@@ -24279,7 +24279,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F24" s="41">
         <v>129</v>
@@ -26342,7 +26342,7 @@
         <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>12</v>
@@ -26351,7 +26351,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F26" s="22">
         <v>18351</v>
@@ -27390,7 +27390,7 @@
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="41" t="s">
         <v>12</v>
@@ -27399,7 +27399,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F27" s="41">
         <v>18351</v>
@@ -28434,7 +28434,7 @@
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" s="41" t="s">
         <v>12</v>
@@ -28443,7 +28443,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F28" s="41">
         <v>18351</v>
@@ -29478,7 +29478,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>12</v>
@@ -29487,7 +29487,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F29" s="41">
         <v>18351</v>
@@ -30522,7 +30522,7 @@
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" s="41" t="s">
         <v>12</v>
@@ -30531,7 +30531,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F30" s="41">
         <v>18351</v>
@@ -31568,7 +31568,7 @@
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="41" t="s">
         <v>12</v>
@@ -31577,7 +31577,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F31" s="41">
         <v>18351</v>
@@ -32612,7 +32612,7 @@
         <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="41" t="s">
         <v>12</v>
@@ -32621,7 +32621,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F32" s="41">
         <v>18351</v>
@@ -33656,7 +33656,7 @@
         <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" s="41" t="s">
         <v>12</v>
@@ -33665,7 +33665,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F33" s="41">
         <v>18351</v>
@@ -34700,7 +34700,7 @@
         <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="41" t="s">
         <v>12</v>
@@ -34709,7 +34709,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F34" s="41">
         <v>18351</v>
@@ -36767,10 +36767,10 @@
     </row>
     <row r="36" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>12</v>
@@ -36779,10 +36779,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G36" s="39" t="s">
         <v>52</v>
@@ -37815,10 +37815,10 @@
     </row>
     <row r="37" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" s="41" t="s">
         <v>12</v>
@@ -37827,10 +37827,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G37" s="39" t="s">
         <v>40</v>
@@ -38859,10 +38859,10 @@
     </row>
     <row r="38" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" s="41" t="s">
         <v>12</v>
@@ -38871,10 +38871,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G38" s="47" t="s">
         <v>41</v>
@@ -39903,10 +39903,10 @@
     </row>
     <row r="39" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>12</v>
@@ -39915,10 +39915,10 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G39" s="39" t="s">
         <v>53</v>
@@ -41973,10 +41973,10 @@
     </row>
     <row r="41" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>12</v>
@@ -41985,10 +41985,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G41" s="39" t="s">
         <v>52</v>
@@ -43021,10 +43021,10 @@
     </row>
     <row r="42" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C42" s="41" t="s">
         <v>12</v>
@@ -43033,10 +43033,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G42" s="39" t="s">
         <v>40</v>
@@ -44065,10 +44065,10 @@
     </row>
     <row r="43" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C43" s="41" t="s">
         <v>12</v>
@@ -44077,10 +44077,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G43" s="47" t="s">
         <v>41</v>
@@ -45109,10 +45109,10 @@
     </row>
     <row r="44" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C44" s="41" t="s">
         <v>12</v>
@@ -45121,10 +45121,10 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G44" s="39" t="s">
         <v>53</v>
@@ -47179,10 +47179,10 @@
     </row>
     <row r="46" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>12</v>
@@ -47191,10 +47191,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G46" s="39" t="s">
         <v>52</v>
@@ -48227,10 +48227,10 @@
     </row>
     <row r="47" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C47" s="41" t="s">
         <v>12</v>
@@ -48239,10 +48239,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F47" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G47" s="39" t="s">
         <v>40</v>
@@ -49271,10 +49271,10 @@
     </row>
     <row r="48" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C48" s="41" t="s">
         <v>12</v>
@@ -49283,10 +49283,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F48" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G48" s="47" t="s">
         <v>41</v>
@@ -50315,10 +50315,10 @@
     </row>
     <row r="49" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C49" s="41" t="s">
         <v>12</v>
@@ -50327,10 +50327,10 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F49" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G49" s="39" t="s">
         <v>53</v>
@@ -52385,10 +52385,10 @@
     </row>
     <row r="51" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>12</v>
@@ -52397,10 +52397,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G51" s="39" t="s">
         <v>52</v>
@@ -53433,10 +53433,10 @@
     </row>
     <row r="52" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C52" s="41" t="s">
         <v>12</v>
@@ -53445,10 +53445,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F52" s="41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G52" s="39" t="s">
         <v>40</v>
@@ -54477,10 +54477,10 @@
     </row>
     <row r="53" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>12</v>
@@ -54489,10 +54489,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F53" s="41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G53" s="47" t="s">
         <v>41</v>
@@ -55521,10 +55521,10 @@
     </row>
     <row r="54" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C54" s="41" t="s">
         <v>12</v>
@@ -55533,10 +55533,10 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F54" s="41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G54" s="39" t="s">
         <v>53</v>
@@ -57591,10 +57591,10 @@
     </row>
     <row r="56" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C56" s="22" t="s">
         <v>12</v>
@@ -57603,10 +57603,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G56" s="39" t="s">
         <v>52</v>
@@ -58639,10 +58639,10 @@
     </row>
     <row r="57" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C57" s="41" t="s">
         <v>12</v>
@@ -58651,10 +58651,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F57" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G57" s="39" t="s">
         <v>40</v>
@@ -59683,10 +59683,10 @@
     </row>
     <row r="58" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C58" s="41" t="s">
         <v>12</v>
@@ -59695,10 +59695,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F58" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G58" s="47" t="s">
         <v>41</v>
@@ -60727,10 +60727,10 @@
     </row>
     <row r="59" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C59" s="41" t="s">
         <v>12</v>
@@ -60739,10 +60739,10 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F59" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G59" s="39" t="s">
         <v>53</v>
@@ -62797,10 +62797,10 @@
     </row>
     <row r="61" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>12</v>
@@ -62809,10 +62809,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G61" s="39" t="s">
         <v>52</v>
@@ -63845,10 +63845,10 @@
     </row>
     <row r="62" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C62" s="41" t="s">
         <v>12</v>
@@ -63857,10 +63857,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F62" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G62" s="39" t="s">
         <v>40</v>
@@ -64889,10 +64889,10 @@
     </row>
     <row r="63" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C63" s="41" t="s">
         <v>12</v>
@@ -64901,10 +64901,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F63" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G63" s="47" t="s">
         <v>41</v>
@@ -65933,10 +65933,10 @@
     </row>
     <row r="64" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C64" s="41" t="s">
         <v>12</v>
@@ -65945,10 +65945,10 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G64" s="39" t="s">
         <v>53</v>
@@ -68003,10 +68003,10 @@
     </row>
     <row r="66" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>12</v>
@@ -68015,10 +68015,10 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G66" s="39" t="s">
         <v>52</v>
@@ -69051,10 +69051,10 @@
     </row>
     <row r="67" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C67" s="41" t="s">
         <v>12</v>
@@ -69063,10 +69063,10 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G67" s="39" t="s">
         <v>40</v>
@@ -70095,10 +70095,10 @@
     </row>
     <row r="68" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C68" s="41" t="s">
         <v>12</v>
@@ -70107,10 +70107,10 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G68" s="47" t="s">
         <v>41</v>
@@ -71139,10 +71139,10 @@
     </row>
     <row r="69" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C69" s="41" t="s">
         <v>12</v>
@@ -71151,10 +71151,10 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G69" s="39" t="s">
         <v>53</v>
@@ -73209,10 +73209,10 @@
     </row>
     <row r="71" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>12</v>
@@ -73221,10 +73221,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F71" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G71" s="39" t="s">
         <v>52</v>
@@ -74257,10 +74257,10 @@
     </row>
     <row r="72" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C72" s="41" t="s">
         <v>12</v>
@@ -74269,10 +74269,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G72" s="39" t="s">
         <v>40</v>
@@ -75301,10 +75301,10 @@
     </row>
     <row r="73" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C73" s="41" t="s">
         <v>12</v>
@@ -75313,10 +75313,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G73" s="47" t="s">
         <v>41</v>
@@ -76345,10 +76345,10 @@
     </row>
     <row r="74" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C74" s="41" t="s">
         <v>12</v>
@@ -76357,10 +76357,10 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G74" s="39" t="s">
         <v>53</v>
@@ -78415,10 +78415,10 @@
     </row>
     <row r="76" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B76" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C76" s="22" t="s">
         <v>12</v>
@@ -78427,10 +78427,10 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F76" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G76" s="39" t="s">
         <v>52</v>
@@ -79463,10 +79463,10 @@
     </row>
     <row r="77" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C77" s="41" t="s">
         <v>12</v>
@@ -79475,10 +79475,10 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F77" s="41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G77" s="39" t="s">
         <v>40</v>
@@ -80507,10 +80507,10 @@
     </row>
     <row r="78" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C78" s="41" t="s">
         <v>12</v>
@@ -80519,10 +80519,10 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F78" s="41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G78" s="47" t="s">
         <v>41</v>
@@ -81551,10 +81551,10 @@
     </row>
     <row r="79" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C79" s="41" t="s">
         <v>12</v>
@@ -81563,10 +81563,10 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F79" s="41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G79" s="39" t="s">
         <v>53</v>
@@ -83621,10 +83621,10 @@
     </row>
     <row r="81" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C81" s="48" t="s">
         <v>12</v>
@@ -83633,10 +83633,10 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F81" s="48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G81" s="49" t="s">
         <v>52</v>
@@ -83654,10 +83654,10 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C82" s="52" t="s">
         <v>12</v>
@@ -83666,10 +83666,10 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F82" s="52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G82" s="39" t="s">
         <v>40</v>
@@ -83683,10 +83683,10 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C83" s="52" t="s">
         <v>12</v>
@@ -83695,10 +83695,10 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F83" s="52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G83" s="47" t="s">
         <v>41</v>
@@ -83712,10 +83712,10 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C84" s="52" t="s">
         <v>12</v>
@@ -83724,10 +83724,10 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F84" s="52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G84" s="39" t="s">
         <v>53</v>
@@ -83752,10 +83752,10 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B86" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C86" s="22" t="s">
         <v>12</v>
@@ -83764,10 +83764,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F86" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G86" s="39" t="s">
         <v>52</v>
@@ -83785,10 +83785,10 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C87" s="41" t="s">
         <v>12</v>
@@ -83797,10 +83797,10 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F87" s="41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G87" s="39" t="s">
         <v>40</v>
@@ -83814,10 +83814,10 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B88" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C88" s="41" t="s">
         <v>12</v>
@@ -83826,10 +83826,10 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F88" s="41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G88" s="47" t="s">
         <v>41</v>
@@ -83843,10 +83843,10 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B89" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C89" s="41" t="s">
         <v>12</v>
@@ -83855,10 +83855,10 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F89" s="41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G89" s="39" t="s">
         <v>53</v>
@@ -83883,10 +83883,10 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B91" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C91" s="22" t="s">
         <v>12</v>
@@ -83895,10 +83895,10 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F91" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G91" s="39" t="s">
         <v>52</v>
@@ -83916,10 +83916,10 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B92" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C92" s="41" t="s">
         <v>12</v>
@@ -83928,10 +83928,10 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F92" s="41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G92" s="39" t="s">
         <v>40</v>
@@ -83943,10 +83943,10 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C93" s="41" t="s">
         <v>12</v>
@@ -83955,10 +83955,10 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F93" s="41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G93" s="47" t="s">
         <v>41</v>
@@ -83970,10 +83970,10 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C94" s="41" t="s">
         <v>12</v>
@@ -83982,10 +83982,10 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F94" s="41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G94" s="39" t="s">
         <v>53</v>
@@ -84000,10 +84000,10 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="B96" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>12</v>
@@ -84012,7 +84012,7 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F96" s="3">
         <v>11690</v>
@@ -84032,10 +84032,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="B98" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>12</v>
@@ -84044,7 +84044,7 @@
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F98" s="3">
         <v>12372</v>

</xml_diff>